<commit_message>
support keywords, disciplines and add better support for alternative locales
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\tsvConversion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajnyga\Documents\GitHub\tsvConverter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="8484"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="1872" windowHeight="6480"/>
   </bookViews>
   <sheets>
     <sheet name="Esimerkki" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="75">
   <si>
     <t>prefix</t>
   </si>
@@ -228,6 +228,27 @@
   </si>
   <si>
     <t>Tämä on sama suomeksi</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>fi</t>
+  </si>
+  <si>
+    <t>Artikkeli suomeksi</t>
+  </si>
+  <si>
+    <t>Tämä artikkeli on suomeksi</t>
+  </si>
+  <si>
+    <t>35-45</t>
+  </si>
+  <si>
+    <t>Tieteellisten seurain valtuuskunta</t>
+  </si>
+  <si>
+    <t>2017-2-2-1.pdf</t>
   </si>
 </sst>
 </file>
@@ -561,30 +582,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB4"/>
+  <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="24.21875" customWidth="1"/>
     <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="13" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" customWidth="1"/>
-    <col min="13" max="14" width="8.88671875" style="2"/>
-    <col min="15" max="15" width="13.44140625" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" customWidth="1"/>
-    <col min="17" max="17" width="16.109375" customWidth="1"/>
-    <col min="18" max="18" width="13.33203125" customWidth="1"/>
-    <col min="19" max="19" width="13.44140625" customWidth="1"/>
-    <col min="20" max="20" width="16.33203125" customWidth="1"/>
-    <col min="23" max="24" width="12.44140625" customWidth="1"/>
+    <col min="4" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="13" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" customWidth="1"/>
+    <col min="14" max="15" width="8.88671875" style="2"/>
+    <col min="16" max="16" width="13.44140625" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" customWidth="1"/>
+    <col min="18" max="18" width="16.109375" customWidth="1"/>
+    <col min="19" max="19" width="13.33203125" customWidth="1"/>
+    <col min="20" max="20" width="13.44140625" customWidth="1"/>
+    <col min="21" max="21" width="16.33203125" customWidth="1"/>
+    <col min="24" max="25" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -600,77 +621,80 @@
       <c r="E1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -683,77 +707,77 @@
       <c r="D2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>42808</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>29</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>1</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>2017</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>25</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>26</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>28</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>30</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>45</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>46</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>47</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>36</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>31</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>20</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>52</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>37</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>39</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>38</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>40</v>
       </c>
@@ -763,56 +787,56 @@
       <c r="D3" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>42808</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>29</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>2017</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>25</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>43</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>48</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>49</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>50</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>51</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>31</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>20</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>61</v>
       </c>
@@ -822,47 +846,103 @@
       <c r="E4" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>42885</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>29</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>2</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>2017</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>26</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>62</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>63</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>64</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>31</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>20</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="1">
+        <v>42885</v>
+      </c>
+      <c r="H5">
+        <v>29</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>2017</v>
+      </c>
+      <c r="L5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="P5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>29</v>
+      </c>
+      <c r="R5" t="s">
+        <v>73</v>
+      </c>
+      <c r="V5" t="s">
+        <v>74</v>
+      </c>
+      <c r="W5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X5" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed trailing space in Data Set in fileGenre2 cell which caused a failed import
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajnyga\Documents\GitHub\tsvConverter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbest/Desktop/JBRIT_import/tsvConverter/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E121FD0-5D37-D141-B3DC-92B908237333}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="1872" windowHeight="6480"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23160" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Esimerkki" sheetId="2" r:id="rId1"/>
@@ -140,9 +141,6 @@
     <t>2017-1-1-2.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Set </t>
-  </si>
-  <si>
     <t>Data set 1</t>
   </si>
   <si>
@@ -249,12 +247,15 @@
   </si>
   <si>
     <t>2017-2-2-1.pdf</t>
+  </si>
+  <si>
+    <t>Data Set</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -304,7 +305,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -581,31 +582,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="Z5" sqref="Z5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.21875" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
     <col min="4" max="6" width="19" customWidth="1"/>
     <col min="7" max="7" width="13" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.21875" customWidth="1"/>
-    <col min="14" max="15" width="8.88671875" style="2"/>
-    <col min="16" max="16" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" customWidth="1"/>
+    <col min="14" max="15" width="8.83203125" style="2"/>
+    <col min="16" max="16" width="13.5" customWidth="1"/>
     <col min="17" max="17" width="13.6640625" customWidth="1"/>
-    <col min="18" max="18" width="16.109375" customWidth="1"/>
+    <col min="18" max="18" width="16.1640625" customWidth="1"/>
     <col min="19" max="19" width="13.33203125" customWidth="1"/>
-    <col min="20" max="20" width="13.44140625" customWidth="1"/>
+    <col min="20" max="20" width="13.5" customWidth="1"/>
     <col min="21" max="21" width="16.33203125" customWidth="1"/>
-    <col min="24" max="25" width="12.44140625" customWidth="1"/>
+    <col min="24" max="25" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -619,10 +620,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>4</v>
@@ -649,7 +650,7 @@
         <v>11</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>12</v>
@@ -679,7 +680,7 @@
         <v>19</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Z1" s="3" t="s">
         <v>33</v>
@@ -691,10 +692,10 @@
         <v>35</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -729,10 +730,10 @@
         <v>27</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P2" t="s">
         <v>28</v>
@@ -744,13 +745,13 @@
         <v>30</v>
       </c>
       <c r="S2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" t="s">
         <v>45</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>46</v>
-      </c>
-      <c r="U2" t="s">
-        <v>47</v>
       </c>
       <c r="V2" t="s">
         <v>36</v>
@@ -762,30 +763,30 @@
         <v>20</v>
       </c>
       <c r="Y2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Z2" t="s">
         <v>37</v>
       </c>
       <c r="AA2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>39</v>
       </c>
-      <c r="AB2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>40</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>41</v>
-      </c>
-      <c r="D3" t="s">
-        <v>42</v>
       </c>
       <c r="G3" s="1">
         <v>42808</v>
@@ -803,28 +804,28 @@
         <v>25</v>
       </c>
       <c r="L3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" t="s">
         <v>43</v>
       </c>
-      <c r="M3" t="s">
-        <v>44</v>
-      </c>
       <c r="N3" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q3" t="s">
         <v>48</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>49</v>
       </c>
-      <c r="R3" t="s">
+      <c r="V3" t="s">
         <v>50</v>
-      </c>
-      <c r="V3" t="s">
-        <v>51</v>
       </c>
       <c r="W3" t="s">
         <v>31</v>
@@ -833,18 +834,18 @@
         <v>20</v>
       </c>
       <c r="Y3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" t="s">
         <v>66</v>
-      </c>
-      <c r="E4" t="s">
-        <v>67</v>
       </c>
       <c r="G4" s="1">
         <v>42885</v>
@@ -865,19 +866,19 @@
         <v>27</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q4" t="s">
         <v>62</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="V4" t="s">
         <v>63</v>
-      </c>
-      <c r="V4" t="s">
-        <v>64</v>
       </c>
       <c r="W4" t="s">
         <v>31</v>
@@ -886,18 +887,18 @@
         <v>20</v>
       </c>
       <c r="Y4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
         <v>70</v>
       </c>
-      <c r="D5" t="s">
-        <v>71</v>
-      </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G5" s="1">
         <v>42885</v>
@@ -918,10 +919,10 @@
         <v>27</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P5" t="s">
         <v>28</v>
@@ -930,10 +931,10 @@
         <v>29</v>
       </c>
       <c r="R5" t="s">
+        <v>72</v>
+      </c>
+      <c r="V5" t="s">
         <v>73</v>
-      </c>
-      <c r="V5" t="s">
-        <v>74</v>
       </c>
       <c r="W5" t="s">
         <v>31</v>
@@ -942,7 +943,7 @@
         <v>20</v>
       </c>
       <c r="Y5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>